<commit_message>
update web 2 0
</commit_message>
<xml_diff>
--- a/private/concepts/seo/WEB_2_0_RESSOURCES_1.xlsx
+++ b/private/concepts/seo/WEB_2_0_RESSOURCES_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\lolvvv1\private\concepts\seo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5401CA67-262B-4B84-9BD5-5E6569B29E00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80510C78-29C7-4FB6-B160-3C9B2ABC7AC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2010" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{EEE84A4D-C1AC-47B8-B08E-7E70A7738F99}"/>
+    <workbookView xWindow="-26025" yWindow="5115" windowWidth="21600" windowHeight="12735" activeTab="1" xr2:uid="{EEE84A4D-C1AC-47B8-B08E-7E70A7738F99}"/>
   </bookViews>
   <sheets>
     <sheet name="Sites" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="74">
   <si>
     <t>probuilds-de</t>
   </si>
@@ -236,6 +236,27 @@
   </si>
   <si>
     <t>https://lolesports.com/article/reflections-on-the-meta-%E2%80%93-into-the-mid-lane-with-humanoid-and-febiven/bltd43ab3abd7ed9d28</t>
+  </si>
+  <si>
+    <t>https://lolesports.com/article/%E2%80%9Cit-can-get-really-brutal%E2%80%9D-%E2%80%93-what-do-the-pros-think-of-yuumi/bltbc4c66cd3645937a</t>
+  </si>
+  <si>
+    <t>not posted yet</t>
+  </si>
+  <si>
+    <t>https://lolesports.com/article/meta-reflection-into-the-jungle-with-sk-trick,-mad-shadow,-and-rge-inspired/blt7a7054fa7a9631af</t>
+  </si>
+  <si>
+    <t>https://lolesports.com/article/mad-kaiser-and-rge-vander-break-down-this-season's-support-meta/blte7822744fe3306f2</t>
+  </si>
+  <si>
+    <t>https://lolesports.com/article/%E2%80%9Ci-hope-the-meta-will-change-every-season%E2%80%9D-%E2%80%93-analysing-the-summer-season-mid-lane-with-mad-humanoid/blted96f359ec766296</t>
+  </si>
+  <si>
+    <t>https://lolesports.com/article/%E2%80%9Ci-liked-the-meta-more-than-in-spring%E2%80%9D-%E2%80%93-reflecting-on-summer-season%E2%80%99s-top-lane-with-mad-lions%E2%80%99-orome/blte7d733406124c06c</t>
+  </si>
+  <si>
+    <t>https://build-de.blogspot.com/2021/01/yuumi-build-playstyle-was-halten-die.html</t>
   </si>
 </sst>
 </file>
@@ -936,13 +957,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7112180D-2353-4EA3-A5BA-B8A536E10350}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,6 +1315,75 @@
       </c>
       <c r="E15" s="5">
         <v>44199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16" t="str">
+        <f>VLOOKUP(A16,Sites!A:C,3,0)</f>
+        <v>de</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="5">
+        <v>44203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17" t="str">
+        <f>VLOOKUP(A17,Sites!A:C,3,0)</f>
+        <v>de</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="e">
+        <f>VLOOKUP(A18,Sites!A:C,3,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="e">
+        <f>VLOOKUP(A19,Sites!A:C,3,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="e">
+        <f>VLOOKUP(A20,Sites!A:C,3,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1314,6 +1404,12 @@
     <hyperlink ref="C8" r:id="rId14" xr:uid="{56FDC5EA-5EC5-46FF-96D9-48B393CCDBDE}"/>
     <hyperlink ref="C15" r:id="rId15" xr:uid="{0C53E77E-B06D-4443-8FA7-20820DEB25AD}"/>
     <hyperlink ref="D15" r:id="rId16" xr:uid="{98AA11DA-6E4F-465D-AA00-C64220270114}"/>
+    <hyperlink ref="D16" r:id="rId17" xr:uid="{E87349E2-8E6E-417A-B523-CD12C22DB2DC}"/>
+    <hyperlink ref="D17" r:id="rId18" xr:uid="{8594F124-0981-4418-945E-8D2744CB504B}"/>
+    <hyperlink ref="D18" r:id="rId19" xr:uid="{7AA658F0-0D93-4655-AEAD-116B1416CCFD}"/>
+    <hyperlink ref="D19" r:id="rId20" xr:uid="{3A5AEBDA-3EB7-4A0E-AD99-F2F6422A8869}"/>
+    <hyperlink ref="D20" r:id="rId21" xr:uid="{333EE67E-1AA6-40AD-9918-14CDB9854AF2}"/>
+    <hyperlink ref="C16" r:id="rId22" xr:uid="{757F35A5-6E82-4268-B933-7D64A3C5362E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
web 2 0 update
</commit_message>
<xml_diff>
--- a/private/concepts/seo/WEB_2_0_RESSOURCES_1.xlsx
+++ b/private/concepts/seo/WEB_2_0_RESSOURCES_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\lolvvv1\private\concepts\seo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C540EF-2627-4ACF-9D92-7682D7827D2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782D3A3D-9E02-4796-BE7F-0C70A7A25B96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{EEE84A4D-C1AC-47B8-B08E-7E70A7738F99}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{EEE84A4D-C1AC-47B8-B08E-7E70A7738F99}"/>
   </bookViews>
   <sheets>
     <sheet name="Sites" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="77">
   <si>
     <t>probuilds-de</t>
   </si>
@@ -241,9 +241,6 @@
     <t>https://lolesports.com/article/%E2%80%9Cit-can-get-really-brutal%E2%80%9D-%E2%80%93-what-do-the-pros-think-of-yuumi/bltbc4c66cd3645937a</t>
   </si>
   <si>
-    <t>not posted yet</t>
-  </si>
-  <si>
     <t>https://lolesports.com/article/meta-reflection-into-the-jungle-with-sk-trick,-mad-shadow,-and-rge-inspired/blt7a7054fa7a9631af</t>
   </si>
   <si>
@@ -262,7 +259,13 @@
     <t>https://build-pt.tumblr.com/post/639695590708707328/syndra-build-orianna-build-analisando-a-pista</t>
   </si>
   <si>
-    <t>In Queue</t>
+    <t>https://buildpl.wordpress.com/2021/01/08/ornn-build-i-renekton-build-refleksja-na-top-lane/</t>
+  </si>
+  <si>
+    <t>https://build-pt.tumblr.com/post/639740051705708544/nautilus-build-yuumi-build-mad-kaiser-e-rge?is_related_post=1</t>
+  </si>
+  <si>
+    <t>https://buildpl.wordpress.com/2021/01/10/sett-build-refleksja-na-junglerzy/</t>
   </si>
 </sst>
 </file>
@@ -649,7 +652,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,7 +972,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
+      <selection pane="bottomRight" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1332,7 +1335,7 @@
         <v>de</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>67</v>
@@ -1349,11 +1352,14 @@
         <f>VLOOKUP(A17,Sites!A:C,3,0)</f>
         <v>pt</v>
       </c>
+      <c r="C17" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="D17" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" t="s">
-        <v>75</v>
+        <v>69</v>
+      </c>
+      <c r="E17" s="5">
+        <v>44204</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1365,37 +1371,49 @@
         <v>pt</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E18" s="5">
         <v>44204</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="e">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19" t="str">
         <f>VLOOKUP(A19,Sites!A:C,3,0)</f>
-        <v>#N/A</v>
+        <v>pl</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="5">
+        <v>44204</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20" t="str">
+        <f>VLOOKUP(A20,Sites!A:C,3,0)</f>
+        <v>pl</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" t="e">
-        <f>VLOOKUP(A20,Sites!A:C,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" t="s">
-        <v>68</v>
+      <c r="E20" s="5">
+        <v>44206</v>
       </c>
     </row>
   </sheetData>
@@ -1423,6 +1441,9 @@
     <hyperlink ref="C16" r:id="rId21" xr:uid="{757F35A5-6E82-4268-B933-7D64A3C5362E}"/>
     <hyperlink ref="C18" r:id="rId22" xr:uid="{4FF5B328-BEAE-40A6-9904-F4E8735D1725}"/>
     <hyperlink ref="D20" r:id="rId23" xr:uid="{2998D0B8-2670-4BD9-BFE0-099E34AC7EED}"/>
+    <hyperlink ref="C19" r:id="rId24" xr:uid="{4CDB4226-983B-4423-BD85-2E20EA96305B}"/>
+    <hyperlink ref="C17" r:id="rId25" xr:uid="{59D2F1EA-E286-4428-A8EA-6C4FF9DB5698}"/>
+    <hyperlink ref="C20" r:id="rId26" xr:uid="{7F69816C-C253-4718-BC52-7D0618442902}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>